<commit_message>
Show temples layer on map
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/файл Ильи.xlsx
+++ b/loadDatabase/religion/файл Ильи.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Лист3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$J$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$J$86</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="564">
   <si>
     <t>Город</t>
   </si>
@@ -1511,12 +1511,251 @@
   </si>
   <si>
     <t>Независимось Грузии</t>
+  </si>
+  <si>
+    <t>Болгария</t>
+  </si>
+  <si>
+    <t>Плиска</t>
+  </si>
+  <si>
+    <t>Создание Болгарского царства</t>
+  </si>
+  <si>
+    <t>после того, как славяне установили власть над Фракией, прибыла новая волна переселенцев, которых называли болгарами. Прекрасные конники и хитроумные политики, болгары тем не менее характеризовались в византийских депешах как «грубые варвары». Они происходили из земель к востоку от Черного моря (возможно, из каспийских степей), но затем прошли вдоль Черноморского побережья и вторглись в Фракию через дельту Дуная. Около 250 000 болгар под командованием хана Аспаруха в 681 г. основали первое болгарское царство со столицей в Плиске.</t>
+  </si>
+  <si>
+    <t>https://wikiway.com/bolgaria/istoriya-bolgarii/</t>
+  </si>
+  <si>
+    <t>Исакча (Румыния)</t>
+  </si>
+  <si>
+    <t>Победа протоболгар над Византией</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Константин IV расположил пехоту между реками Ольгою и Дунаем, а корабли поставил у берегов реки. Булгары, увидев многочисленность византийского войска, нашли убежище в своих деревянных укреплениях. Осада, затруднённая болотистостью здешней местности, продолжалась три или четыре дня[2]. 
+Так как византийцы не начинали сражения, булгары стали смелее и сами начали атаковать противника. Константин IV страдал от подагры и был вынужден возвратиться на юг для пользования минеральными банями (возможно, в Бургасе). Византийская армия посчитала этот отъезд императора бегством с поля боя. Вслед за этим в её рядах начались беспорядки. Воспользовавшись ими, булгары напали на византийцев. Феофан Исповедник сообщал: «Болгары уже приметивши это, преследовали их, весьма многих истребили мечом, многих ранили, гнались за ними до самого Дуная, переправились чрез эту реку
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%B8%D1%82%D0%B2%D0%B0_%D0%BF%D1%80%D0%B8_%D0%9E%D0%BD%D0%B3%D0%B0%D0%BB%D0%B5</t>
+  </si>
+  <si>
+    <t>Требине</t>
+  </si>
+  <si>
+    <t>Ведшая территориальную экспансию Болгария, подчинила Срем и часть правобережья Дуная, после чего попыталась завоевать и Сербию. В этом конфликте сербам помогла Византия: император Феофил оказал им поддержку и пообещал признать их независимость сразу же после победы над болгарами[1]. Согласно Константину Багрянородному, болгары планировали завоевать страну окончательно, принуждая различными способами сербов подчиниться. В 839 году болгарский хан Пресиан (правил в 836—852 годах) вторгся в Сербию. В 842 году Пресиан был полностью разбит, его армия практически уничтожена, а сам он возвратился в свои владения ни с чем.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%92%D0%BB%D0%B0%D1%81%D1%82%D0%B8%D0%BC%D0%B8%D1%80</t>
+  </si>
+  <si>
+    <t>Начало крещения болгар</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Борис принял решение в начале 860-х годов о принятии христианства своим народом и сам около 865 года был крещён под именем Михаила — в честь своего крестного отца — византийского императора Михаила III. Продолжатель Феофана отмечал личную роль Феодоры в деле христианизации Болгарии, хотя, следуя агиографической традиции, основную причину крещения видит в избавлении болгар с помощью Бога от сильного голода. Причины принятия христианства могли быть глубже. Во-первых, языческая религия мешала Болгарии во внешней политике, потому что все страны, с которыми Болгария заключала договоры, были христианскими, — а разница в религиях очень часто использовалась как предлог для нарушения уже заключенных договоров. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%BE%D1%80%D0%B8%D1%81_I</t>
+  </si>
+  <si>
+    <t>27/05/927</t>
+  </si>
+  <si>
+    <t>Вишеград</t>
+  </si>
+  <si>
+    <t>Согласно источникам, описывающим ход битвы, войско хорватского короля полностью опустошило болгарские войска. Решающим фактором для победы хорватов был верно выбранный ландшафт — хорваты базировались на холмах. Хорватские воины были также лучше вооружены и, конечно же, их численность превосходила силы противника более чем вдвое. Наконец сказался и человеческий фактор: когда основные силы болгар были разбиты, Томислав лично возглавил конницу и нанес решающий удар по противнику</t>
+  </si>
+  <si>
+    <t>Битва Болгар и Хорватов</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%B8%D1%82%D0%B2%D0%B0_%D0%BD%D0%B0_%D0%B1%D0%BE%D1%81%D0%BD%D0%B8%D0%B9%D1%81%D0%BA%D0%B8%D1%85_%D1%85%D0%BE%D0%BB%D0%BC%D0%B0%D1%85</t>
+  </si>
+  <si>
+    <t>Силистра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Святослав привёл 60 тысяч воинов и начал свою кампанию на Дунае только в начале весны 968 года. Столкновение с болгарским войском, насчитывавшим 30 тысяч человек, произошло близ Доростола. Бой продолжался весь день. В результате болгары были разбиты и отступили к Доростолу, выдержав в нём осаду. </t>
+  </si>
+  <si>
+    <t>Битва Болгарского и русского войска</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%B8%D1%82%D0%B2%D0%B0_%D0%BF%D1%80%D0%B8_%D0%94%D0%BE%D1%80%D0%BE%D1%81%D1%82%D0%BE%D0%BB%D0%B5_(968)</t>
+  </si>
+  <si>
+    <t>Во время осады Диррахия в 1018 году болгарский правитель Иван Владислав был убит. Василий II с триумфом въехал в столицу завоёванной страны — Охрид, и приказал сравнять городские стены с землёй[47]. После победы над болгарами венгры и византийцы разделили между собой почти все захваченные земли: венгры заняли территории к северо-западу от Карпат, а византийцы — к югу от Дуная. Северо-восточные земли за Дунаем остались за печенегами[45]. Наиболее именитых боляр Василий II переселил в Византию, в основном в Малую Азию. Большая же часть болгарской знати осталась на родине, сохранив своё положение и имущество</t>
+  </si>
+  <si>
+    <t>Дуррес (Албания)</t>
+  </si>
+  <si>
+    <t>Победа Венгерско-Византийского войска над Болгарией</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%98%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F_%D0%91%D0%BE%D0%BB%D0%B3%D0%B0%D1%80%D0%B8%D0%B8</t>
+  </si>
+  <si>
+    <t>Болгария под властью Византии</t>
+  </si>
+  <si>
+    <t>В Византии вместо прежнего названия «Болгария» в документах и обиходе были введены новые названия — Мизия или Загорье[49]. Болгарская церковь была подчинена Константинопольской церкви[50]. На раньше всех завоёванной Северо-Восточной Болгарии была создана фема Паристрион[en] (то есть Подунавье) или «Поистрийские города». В отдельную фему была выделена Сирмия[en]. В особую административную единицу был выделен Диррахий (Дуррес) с пригородом. Другая часть земель вошла в провинцию (фему) под названием Болгария[en] (юг современной Сербии с прилегающими районами[51]). Северо-Восточная Болгария в конце XI—XII века была заселена кочевыми печенегами и половцами, враждебными по отношению к Византии. Болгарские земли передавались духовенству, крестьянам, переселившимся из других уголков Византийской империи, а также бывшим кочевникам, оказавшимся в плену. К концу XI века возросли владения византийской знати. Часть юго-западных болгарских земель передавалась императорами в пронии. Бывшие болгарские земли Средней и Южной Македонии в XII веке остались во владениях византийских императоров</t>
+  </si>
+  <si>
+    <t>Адрианополь</t>
+  </si>
+  <si>
+    <t>Победа болгар над крестоносцами</t>
+  </si>
+  <si>
+    <t>41°40′00″ с. ш. 26°34′00″ в. д.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%B8%D1%82%D0%B2%D0%B0_%D0%BF%D0%BE%D0%B4_%D0%90%D0%B4%D1%80%D0%B8%D0%B0%D0%BD%D0%BE%D0%BF%D0%BE%D0%BB%D0%B5%D0%BC_(1205)</t>
+  </si>
+  <si>
+    <t>В этой битве крестоносцы понесли тяжелейшие потери, погибло множество рыцарей, а сам император Балдуин попал в плен, где впоследствии умер насильственной смертью. 1 июня умер участвовавший в походе венецианский дож Энрико Дандоло, чьё тело было захоронено в соборе святой Софии. Поражение полностью уничтожило ореол непобедимости вокруг латинян, до этого компенсировавший их малочисленность. Объединённое войско болгар и половцев расширило ареал грабежа и разбоя до Редеста, Селимврии и Константинополя, хотя из-за этой жестокости от Иоанна позже отпадёт греческое население</t>
+  </si>
+  <si>
+    <t>В 1242 году Болгария подверглась разорению монголо-татарами, превратившись в их данника. После этого события в стране более чем на полвека развернулись междоусобные войны, во время которых в Болгарии поменялось восемь правителей. В это время Болгария стала уступать своим соседям в военном превосходстве на Балканах. Войны с Венгрией, Никейской империей и Эпирским царством привели к потере страной территорий в Южной и Средней Македонии, Родопской области, городов Скопье, Охрид, Белград, Ниш и других. В результате сербской экспансии в конце XIII века Болгария навсегда потеряла Македонию</t>
+  </si>
+  <si>
+    <t>Захват Болгарии Монголами</t>
+  </si>
+  <si>
+    <t>Тырново</t>
+  </si>
+  <si>
+    <t>Максимальное могущество Болгарского царства</t>
+  </si>
+  <si>
+    <t>При Иване Асене II (правл. 1218—1241) Болгарское царство временно превратилось в гегемона на Балканах. Он расширил территорию Болгарии, почти бескровно подчинив себе Западную Фракию, Македонию, Западный Эпир и Северную Фессалию. С соседней Сербией Асень сохранял дружеские отношения. На одной из колонн в тырновской церкви Сорока мучеников царь приказал выбить слова: «В лето 6738 (1230)… я, Иван Асень, во Христе боге верный царь и самодержец болгар… в двенадцатый год своего царствования разбил греческие войска, а самого царя, господина Феодора Комнина, взял в плен со всеми его болярами. И взял всю его землю…»[</t>
+  </si>
+  <si>
+    <t>София</t>
+  </si>
+  <si>
+    <t>Осада и взятие турками Софии</t>
+  </si>
+  <si>
+    <t>С наступлением турок к 1373 году Болгария потеряла все владения к югу от Стара-Планины. Иван Шишман был вынужден признать себя вассалом османского султана. В 1380 году турки осадили Софию, которая через два года пала. После нашествия 30-тысячного войска турок Тырновское царство сузилось до столичной округи. После того, как султан узнал о переговорах Ивана Шишмана о союзе с венграми, Тырнов в 1393 году был осаждён турецкой армией. Оставшиеся в живых жители столицы были уведены в рабство или переселены в Малую Азию. Тырнов был заселён турками</t>
+  </si>
+  <si>
+    <t>На всём протяжении турецкого периода в Болгарии существовали отряды гайдуков, нападавшие на турок. В конце XVI века их отряды выросли с нескольких десятков до 600 человек. В 1595 году гайдуки даже захватили Софию. Особенно активны гайдуки были в западных районах Болгарии рядом с горами. Ответные экспедиции турецких карателей заканчивались казнью гайдуков и насильственной исламизацией близлежащих деревень. Во время австро-турецкой войны, начавшейся в 1593 году, по Балканам прокатилась волна восстаний. В ходе Первого Тырновского восстания, вспыхнувшего в 1598 году, Шишман III, якобы потомок династии Шишмановичей, провозгласил себя в Тырнове царём</t>
+  </si>
+  <si>
+    <t>Восстание гайдуков и временное освобождение от турок Софии</t>
+  </si>
+  <si>
+    <t>Ясы</t>
+  </si>
+  <si>
+    <t>29/12/1791</t>
+  </si>
+  <si>
+    <t>Ясский мирный договор</t>
+  </si>
+  <si>
+    <t>Россия получила право покровительства христианских народов Османской империи. В начале XIX века появились греко-болгарские школы, где преподавали болгарскую грамматику, а также арифметику, естествознание и географию. Позднее возникли и чисто болгарские школы</t>
+  </si>
+  <si>
+    <t>Чипровец</t>
+  </si>
+  <si>
+    <t>Чипровское восстание</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A7%D0%B8%D0%BF%D1%80%D0%BE%D0%B2%D1%81%D0%BA%D0%BE%D0%B5_%D0%B2%D0%BE%D1%81%D1%81%D1%82%D0%B0%D0%BD%D0%B8%D0%B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В августе 1688 г архиепископ Стефан Кнежевич, опасаясь актов возмездия против Чипровцев со стороны османов, обратился к австрийскому императору Леопольду I с просьбой о помощи. В ответ к Чипровцам было отправлено шесть артиллерийских полков под командованием генерала Доната Иоганна Хейслера фон Хайтерсхайма, а в авангарде этих сил были кавалерийские роты Пеячевича и Ласло Чаки, а также отряд Маринова. Когда они подошли к регулярной армии, четыре отряда из Чипровцев и Копиловцев объединились, а затем к ним примкнули и другие добровольцы, и их общее количество оценивалось примерно в 20 000 человекОсманские силы из Софии 18 октября достигли района Жеравицы и атаковали повстанцев. Плохое укрепление и пониженная бдительность в лагере дали нападавшим преимущество. Повстанцам пришлось отступить. Они заняли оборону в деревне к северу (ныне не сохранившейся) и тем самым преуменьшили преимущество врага в численности и высокой боевой эффективности. Таким образом, им удалось первоначально справиться с этой атакой. После ещё нескольких отражённых атак их ряды начали серьёзно истощаться, как из-за большого количества жертв, так и от бегства рекрутов из польских деревень. В итоге повстанцы были разбиты османскими войсками и их венгерскими союзниками во главе с графом Имре Тёкёли. </t>
+  </si>
+  <si>
+    <t>Пловдив</t>
+  </si>
+  <si>
+    <t>Авпрельское восстание против Осман</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Несмотря на поражение, Апрельское восстание поколебало турецкое феодальное господство в Болгарии, а жестокое подавление восстания привлекло внимание великих держав (в первую очередь, Великобритании[14] и Российской империи[14]) к событиям на Балканах[7], стало предметом рассмотрения на Константинопольской конференции и одной из причин русско-турецкой войны 1877—1878 годов, в результате которой Болгария была освобождена от турецкого господства. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%90%D0%BF%D1%80%D0%B5%D0%BB%D1%8C%D1%81%D0%BA%D0%BE%D0%B5_%D0%B2%D0%BE%D1%81%D1%81%D1%82%D0%B0%D0%BD%D0%B8%D0%B5_(1876)</t>
+  </si>
+  <si>
+    <t>Шипка</t>
+  </si>
+  <si>
+    <t>Русско-Турецкая война</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Россия вернула южную часть Бессарабии, потерянную после Крымской войны, присоединила Карсскую область, населённую армянами и грузинами, и заняла стратегически важную Батумскую область (с условием организовать порто-франко, однако вскоре для защиты города возведена Михайловская крепость). 
+Великобритания оккупировала Кипр, согласно договору с Османской империей от 4 июня 1878 года; в обмен на это она обязалась защищать Турцию от дальнейшего российского продвижения в Закавказье. Оккупация Кипра должна была длиться, пока в руках русских остаются Карс и Батуми[56]. 
+Границы, установленные по итогам войны, сохраняли силу до Балканских войн 1912—1913 годов, с некоторыми изменениями: 
+В 1885 году Княжество Болгария и Восточная Румелия объединились в единое княжество;
+В 1908 году Болгария объявила себя независимым от Турции царством, а Австро-Венгрия аннексировала ранее оккупированную ею Боснию и Герцеговину.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%BE-%D1%82%D1%83%D1%80%D0%B5%D1%86%D0%BA%D0%B0%D1%8F_%D0%B2%D0%BE%D0%B9%D0%BD%D0%B0_(1877%E2%80%941878)</t>
+  </si>
+  <si>
+    <t>5 октября 1908 года в церкви Сорока мучеников в Тырнове была провозглашена независимость Болгарии, превратившейся в царство. За признание независимости Османская империя потребовала от болгар денежную компенсацию в 125 млн франков, из которой 43 млн франков Россия добровольно приняла на себя. Между тем, в Македонии, по болгарским данным 1900 года, проживало 1,181 млн болгар, 499 тысяч турок, 229 тысяч греков, а также албанцы, румыны, евреи, цыгане. В 1870 году православное население Македонии начало переходить под юрисдикцию Болгарской церкви</t>
+  </si>
+  <si>
+    <t>Независимость Болгарии</t>
+  </si>
+  <si>
+    <t>14 октября 1915 года Болгария вступила в войну на стороне Тройственного союза. Болгарская армия повела наступление на Македонию и Сербию. В Вардарской Македонии и Помаравье болгары установили оккупационный режим. 1 сентября 1916 года Болгария объявила войну Румынии, вступившей в войну на стороне Антанты. Россия разорвала отношения с Болгарией и объявила ей войну. Когда в сентябре 1916 года русские воевали против болгар в Добрудже, поэт И. Вазов в своём стихотворении вопрошал: «О, русские, братья славянские, зачем вы здесь?»[89]. К началу 1917 года болгарские войска заняли всю Добруджу до устья Дуная. В течение трёх лет болгары воевали без поражений, пока в сентябре 1918 года не столкнулись на Салоникском фронте с войсками Антанты. Во время Владайского восстания между Болгарией и Антантой 29 сентября было заключено Салоникское перемирие. На следующий день восстание было подавлено[90]. 3 октября царь Фердинанд отрёкся от престола в пользу сына и уехал в Германию[91]. 27 ноября 1919 года был заключён Нёйиский договор, по которому Болгария потеряла ряд западных областей и Западную Фракию</t>
+  </si>
+  <si>
+    <t>Болгария участвует в 1 мировой войне на стороне тройственного союза</t>
+  </si>
+  <si>
+    <t>1 марта 1941 года Болгария подписала Тройственный пакт, условившись не принимать участия в военных действиях. На следующий день 680-тысячная немецкая армия вступила на болгарскую землю для последующего вторжения в Югославию и Грецию. Население встречало немцев с цветами</t>
+  </si>
+  <si>
+    <t>Болгария поддержала Германию во 2 мировой войне</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19-20 апреля 1941 года, в соответствии с соглашением между Германией, Италией и правительством Болгарии, части болгарской армии без объявления войны пересекли границы с Югославией и Грецией и оккупировали территории в Македонии и Северной Греции. 24 мая 1941 года между Болгарией и Италией были подписаны дополнительные соглашения, уточнившие разделение зон оккупации.
+В результате в сентябре 1940—апреле 1941 г. в состав Болгарии вошли 42 466 км² территории с населением 1,9 млн чел[27]. Возникла Великая Болгария от Чёрного до Эгейского моря. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%BE%D0%BB%D0%B3%D0%B0%D1%80%D0%B8%D1%8F_%D0%B2%D0%BE_%D0%92%D1%82%D0%BE%D1%80%D0%BE%D0%B9_%D0%BC%D0%B8%D1%80%D0%BE%D0%B2%D0%BE%D0%B9_%D0%B2%D0%BE%D0%B9%D0%BD%D0%B5</t>
+  </si>
+  <si>
+    <t>Болгария аннексировала Македонию и Северную Грецию</t>
+  </si>
+  <si>
+    <t>Вардар</t>
+  </si>
+  <si>
+    <t>Образование НРБ</t>
+  </si>
+  <si>
+    <t>15 сентября 1946 года после проведения референдума Болгария была провозглашена народной республикой. В ноябре 1946 года правительство возглавил Г. Димитров. 4 декабря 1947 года Великое народное собрание приняло новую конституцию, которая вскоре получила название «Димитровской». После занятия должности генерального секретаря ЦК БКП В. Червенковым решения по всем основным вопросам государства принимались по согласованию со сталинским руководством. Кадровые перестановки производились с привлечением советников из СССР в Софии.</t>
+  </si>
+  <si>
+    <t>Болгария предоставила воздушное простванство НАТО для ударов по Белграду</t>
+  </si>
+  <si>
+    <t>Брюссель</t>
+  </si>
+  <si>
+    <t>Болгария вступила в НАТО</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1576,10 +1815,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1887,13 +2126,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B70" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomRight" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2151,7 +2390,7 @@
       <c r="B10" s="3">
         <v>642</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -2301,7 +2540,7 @@
       <c r="B16" s="3">
         <v>1054</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="6" t="s">
         <v>306</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -3048,7 +3287,7 @@
       <c r="B46" s="3">
         <v>1929</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>10599</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -3103,7 +3342,7 @@
       <c r="B48" s="3">
         <v>1945</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>16770</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -3129,7 +3368,7 @@
       <c r="B49" s="3">
         <v>1992</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D49" s="5">
         <v>33721</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -3155,7 +3394,7 @@
       <c r="B50" s="3">
         <v>2006</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D50" s="5">
         <v>38871</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -3351,6 +3590,12 @@
       <c r="G58" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I58" s="3">
+        <v>1</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="59" spans="1:10" ht="186" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -3368,6 +3613,12 @@
       <c r="G59" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I59" s="3">
+        <v>1</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="60" spans="1:10" ht="162.75" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
@@ -3385,6 +3636,12 @@
       <c r="G60" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I60" s="3">
+        <v>1</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="61" spans="1:10" ht="186" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
@@ -3402,6 +3659,12 @@
       <c r="G61" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I61" s="3">
+        <v>1</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="62" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -3419,6 +3682,12 @@
       <c r="G62" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I62" s="3">
+        <v>1</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="63" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -3436,8 +3705,14 @@
       <c r="G63" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="I63" s="3">
+        <v>1</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>454</v>
       </c>
@@ -3453,8 +3728,14 @@
       <c r="G64" s="3" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="186" x14ac:dyDescent="0.25">
+      <c r="I64" s="3">
+        <v>1</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="186" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>442</v>
       </c>
@@ -3470,8 +3751,14 @@
       <c r="G65" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="I65" s="3">
+        <v>1</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>469</v>
       </c>
@@ -3487,8 +3774,14 @@
       <c r="G66" s="4" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" ht="93" x14ac:dyDescent="0.25">
+      <c r="I66" s="3">
+        <v>1</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="93" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>442</v>
       </c>
@@ -3504,8 +3797,14 @@
       <c r="G67" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="I67" s="3">
+        <v>1</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>474</v>
       </c>
@@ -3524,8 +3823,14 @@
       <c r="G68" s="4" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" ht="139.5" x14ac:dyDescent="0.25">
+      <c r="I68" s="3">
+        <v>1</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="139.5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>483</v>
       </c>
@@ -3544,15 +3849,21 @@
       <c r="G69" s="4" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" ht="372" x14ac:dyDescent="0.25">
+      <c r="I69" s="3">
+        <v>1</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="372" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>442</v>
       </c>
       <c r="B70" s="3">
         <v>1921</v>
       </c>
-      <c r="D70" s="6">
+      <c r="D70" s="5">
         <v>7723</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -3564,15 +3875,21 @@
       <c r="G70" s="3" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="I70" s="3">
+        <v>1</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>442</v>
       </c>
       <c r="B71" s="3">
         <v>1991</v>
       </c>
-      <c r="D71" s="6">
+      <c r="D71" s="5">
         <v>33337</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -3584,9 +3901,607 @@
       <c r="G71" s="4" t="s">
         <v>449</v>
       </c>
+      <c r="I71" s="3">
+        <v>1</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="325.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B72" s="3">
+        <v>680</v>
+      </c>
+      <c r="D72" s="5"/>
+      <c r="E72" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="I72" s="3">
+        <v>1</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B73" s="3">
+        <v>681</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="I73" s="3">
+        <v>1</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B74" s="3">
+        <v>839</v>
+      </c>
+      <c r="C74" s="3">
+        <v>842</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="I74" s="3">
+        <v>1</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="232.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B75" s="3">
+        <v>864</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="I75" s="3">
+        <v>1</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="B76" s="3">
+        <v>927</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="I76" s="3">
+        <v>1</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="93" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B77" s="3">
+        <v>968</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="I77" s="3">
+        <v>1</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1018</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I78" s="3">
+        <v>1</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="348.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1018</v>
+      </c>
+      <c r="C79" s="3">
+        <v>1186</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I79" s="3">
+        <v>1</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1205</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="I80" s="3">
+        <v>1</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1241</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I81" s="3">
+        <v>1</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1242</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="I82" s="3">
+        <v>1</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1380</v>
+      </c>
+      <c r="C83" s="3">
+        <v>1383</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I83" s="3">
+        <v>1</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1595</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I84" s="3">
+        <v>1</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1688</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="I85" s="3">
+        <v>1</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="93" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B86" s="3">
+        <v>1791</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I86" s="3">
+        <v>1</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="139.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1876</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="I87" s="3">
+        <v>1</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="395.25" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B88" s="3">
+        <v>1877</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1878</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="I88" s="3">
+        <v>1</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1908</v>
+      </c>
+      <c r="D89" s="5">
+        <v>3201</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I89" s="3">
+        <v>1</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="348.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1914</v>
+      </c>
+      <c r="C90" s="3">
+        <v>1919</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I90" s="3">
+        <v>1</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="93" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1941</v>
+      </c>
+      <c r="D91" s="5">
+        <v>15036</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I91" s="3">
+        <v>1</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1941</v>
+      </c>
+      <c r="D92" s="5">
+        <v>15085</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="I92" s="3">
+        <v>1</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B93" s="3">
+        <v>1946</v>
+      </c>
+      <c r="D93" s="5">
+        <v>17060</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I93" s="3">
+        <v>1</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1999</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I94" s="3">
+        <v>1</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="B95" s="3">
+        <v>2004</v>
+      </c>
+      <c r="D95" s="5">
+        <v>38075</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="I95" s="3">
+        <v>1</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>488</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J10">
+  <autoFilter ref="A1:J86">
     <sortState ref="A2:G678">
       <sortCondition ref="A1:A376"/>
     </sortState>
@@ -3654,9 +4569,32 @@
     <hyperlink ref="G68" r:id="rId60"/>
     <hyperlink ref="G69" r:id="rId61"/>
     <hyperlink ref="G71" r:id="rId62"/>
+    <hyperlink ref="G73" r:id="rId63"/>
+    <hyperlink ref="G72" r:id="rId64"/>
+    <hyperlink ref="G74" r:id="rId65"/>
+    <hyperlink ref="G75" r:id="rId66"/>
+    <hyperlink ref="G76" r:id="rId67"/>
+    <hyperlink ref="G77" r:id="rId68"/>
+    <hyperlink ref="G78" r:id="rId69"/>
+    <hyperlink ref="G79" r:id="rId70"/>
+    <hyperlink ref="G80" r:id="rId71"/>
+    <hyperlink ref="G81" r:id="rId72"/>
+    <hyperlink ref="G83" r:id="rId73"/>
+    <hyperlink ref="G84" r:id="rId74"/>
+    <hyperlink ref="G86" r:id="rId75"/>
+    <hyperlink ref="G85" r:id="rId76"/>
+    <hyperlink ref="G87" r:id="rId77"/>
+    <hyperlink ref="G88" r:id="rId78"/>
+    <hyperlink ref="G89" r:id="rId79"/>
+    <hyperlink ref="G90" r:id="rId80"/>
+    <hyperlink ref="G91" r:id="rId81"/>
+    <hyperlink ref="G92" r:id="rId82"/>
+    <hyperlink ref="G93" r:id="rId83"/>
+    <hyperlink ref="G94" r:id="rId84"/>
+    <hyperlink ref="G95" r:id="rId85"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId86"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Load and show holy persons in map
</commit_message>
<xml_diff>
--- a/loadDatabase/religion/файл Ильи.xlsx
+++ b/loadDatabase/religion/файл Ильи.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="674">
   <si>
     <t>Город</t>
   </si>
@@ -1747,6 +1747,366 @@
   </si>
   <si>
     <t>Болгария вступила в НАТО</t>
+  </si>
+  <si>
+    <t>Россия</t>
+  </si>
+  <si>
+    <t>02.09.911</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Русско-византийский договор </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Договор устанавливал дружественные отношения Византии и Руси, определял порядок выкупа пленных, наказания за уголовные преступления, совершённые греческими и русскими купцами в Византии, правила ведения судебного процесса и наследования, создавал благоприятные условия торговли для русских и греков, изменял береговое право. Отныне вместо захвата выброшенного на берег судна и его имущества, владельцы берега обязывались оказывать помощь в их спасении. 
+Также по условиям договора русские купцы получили право жить в Константинополе по полгода, империя обязывалась содержать их в течение этого времени за счёт казны. Им было предоставлено право беспошлинной торговли в Византии. И ещё допускалась возможность найма русских на военную службу в Византии. 
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%BE-%D0%B2%D0%B8%D0%B7%D0%B0%D0%BD%D1%82%D0%B8%D0%B9%D1%81%D0%BA%D0%B8%D0%B9_%D0%B4%D0%BE%D0%B3%D0%BE%D0%B2%D0%BE%D1%80_(911)</t>
+  </si>
+  <si>
+    <t>Ладога</t>
+  </si>
+  <si>
+    <t>Княжение Рюрика в Ладоге</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Согласно летописям, в 862 году варяг Рюрик с братьями Синеусом и Трувором по приглашению ильменских словен и кривичей, а также таких племён, как чудь и весь, были призваны княжить в трёх городовых областях. Синеус — в Белоозере, Трувор — в Изборске, а Рюрик по одним данным — в Ладоге, по другим — в Новгороде. Это событие, с которого традиционно отсчитывается начало русской государственности, в историографии получило условное название призвание варягов. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D1%8E%D1%80%D0%B8%D0%BA</t>
+  </si>
+  <si>
+    <t>Киев</t>
+  </si>
+  <si>
+    <t>Крещение Руси</t>
+  </si>
+  <si>
+    <t>В 988 году князь Владимир Великий после похода на византийский Херсонес и женитьбы на сестре византийских императоров Анне утвердил восточное христианство на Руси в качестве государственной религии[42][43]. Принятие христианства укрепляло государственную власть и территориальное единство Древнерусского государства. Оно имело большое международное значение: Русь, отвергнув примитивное язычество, стала теперь равной другим христианским народам.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%98%D1%81%D1%82%D0%BE%D1%80%D0%B8%D1%8F_%D0%A0%D0%BE%D1%81%D1%81%D0%B8%D0%B8</t>
+  </si>
+  <si>
+    <t>Выпуск первого свода законов - "Русской правды"</t>
+  </si>
+  <si>
+    <t>Краткая редакция включает 43 статьи. Первая её часть, наиболее древняя (Правда Ярослава), отмечает сохранение обычая кровной мести, хотя и ограничивает его кругом ближайших родственников[3], отсутствие чёткой дифференциации размеров судебных штрафов в зависимости от социального статуса потерпевшего. Правда Ярославичей отражает дальнейший процесс развития правовых отношений: включает повышенные штрафы за убийство привилегированных слоев общества. Значительная часть статей посвящена защите княжеского хозяйства и княжеских людей. Наказаниями по Краткой Правде являются денежные штрафы, за наиболее тяжкие преступления допускается расправа на месте происшествия. Большинство учёных относят Краткую Правду к XI веку</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%B0%D1%8F_%D0%9F%D1%80%D0%B0%D0%B2%D0%B4%D0%B0</t>
+  </si>
+  <si>
+    <t>Монголо-Татарское нашествие</t>
+  </si>
+  <si>
+    <t>Коломна</t>
+  </si>
+  <si>
+    <t>В ходе монгольского нашествия (1237—1240) русские войска потерпели ряд поражений, многие русские города подверглись разорению. В 1237—1238 годах монголы разгромили северо-восточные русские княжества. Соединённые силы Владимирского и Рязанского княжеств потерпели поражение в битве у Коломны. Владимирский князь Юрий II Всеволодович не смог противостоять монголам и был разбит в битве на реке Сити. В 1239—1240 годах монголы разгромили юго-западные русские земли, взяв Киев в 1240 году. Все русские земли оказались под верховной властью Монгольской империи, в подчинении её западного крыла — Улуса Джучи или Золотой Орды. Верховными арбитрами в спорах за княжения, в том числе за Киев, стали ордынские ханы</t>
+  </si>
+  <si>
+    <t>15/06/1240</t>
+  </si>
+  <si>
+    <t>59°48′27″ с. ш. 30°36′15″ в. д.</t>
+  </si>
+  <si>
+    <t>Усть-Ижора</t>
+  </si>
+  <si>
+    <t>Невская битва</t>
+  </si>
+  <si>
+    <t>Одержав победу над шведами, русские войска остановили их продвижение на Ладогу и Новгород и тем самым предупредили опасность скоординированных действий Швеции и Ордена в ближайшем будущем. 
+Однако из-за страха перед тем, что после победы роль Александра в ведении дел может возрасти, новгородские бояре стали строить князю всевозможные козни. Александр Невский уехал к отцу, но уже через год новгородские жители снова пригласили князя для продолжения войны с Ливонским орденом</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9D%D0%B5%D0%B2%D1%81%D0%BA%D0%B0%D1%8F_%D0%B1%D0%B8%D1%82%D0%B2%D0%B0</t>
+  </si>
+  <si>
+    <t>Вследствие одержанной победы Ольгерд включил в состав своего государства, занимавшего в то время значительные территории по обоим берегам Днепра, Киевское княжество и захваченное татарами ещё в середине XIII века Подолье, расширив таким образом свои владения далеко на юг по направлению к Чёрному морю. Победа Ольгерда и приход на Подолье Кориатовичей укрепили княжество Молдавия</t>
+  </si>
+  <si>
+    <t>Победа Литовского княжества над Ордынскими войсками "на синих водах"</t>
+  </si>
+  <si>
+    <t>48°02′59″ с. ш. 30°50′57″ в. д.</t>
+  </si>
+  <si>
+    <t>Первомайск (Украина)</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%91%D0%B8%D1%82%D0%B2%D0%B0_%D0%BD%D0%B0_%D0%A1%D0%B8%D0%BD%D0%B8%D1%85_%D0%92%D0%BE%D0%B4%D0%B0%D1%85</t>
+  </si>
+  <si>
+    <t>Куликово поле (Ивановка, Тульская область)</t>
+  </si>
+  <si>
+    <t>Куликовская битва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">«победа на Куликовом поле закрепила за Москвой значение организатора и идеологического центра воссоединения восточнославянских земель, показав, что путь к их государственно-политическому единству был единственным путём и к их освобождению от чужеземного господства»[4]. 
+Для самой Орды поражение войска Мамая способствовало её консолидации «под властью единого правителя хана Тохтамыша»[49]. Мамай спешно собрал в Крыму остаток сил, собираясь снова изгоном идти на Русь, но был разбит Тохтамышем. Поскольку Дмитрий отказался от продолжения выплаты дани Тохтамышу, спустя два года после Куликовской битвы золотоордынцы предприняли поход на Москву, сожгли город и принудили Дмитрия возобновить выплату дани
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9A%D1%83%D0%BB%D0%B8%D0%BA%D0%BE%D0%B2%D1%81%D0%BA%D0%B0%D1%8F_%D0%B1%D0%B8%D1%82%D0%B2%D0%B0</t>
+  </si>
+  <si>
+    <t>53°36′23″ с. ш. 38°40′30″ в. д.</t>
+  </si>
+  <si>
+    <t>Шелонская битва</t>
+  </si>
+  <si>
+    <t>14/07/1471</t>
+  </si>
+  <si>
+    <t>Сольцы (Новгородская обл)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> В результате битвы Новгород потерпел тяжёлое поражение, были уничтожены его лучшие воины, что предопределило окончательное поражение Новгородской республики и подчинение её Москве в ходе следующей московско-новгородской войны 1477—1478 года. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A8%D0%B5%D0%BB%D0%BE%D0%BD%D1%81%D0%BA%D0%B0%D1%8F_%D0%B1%D0%B8%D1%82%D0%B2%D0%B0</t>
+  </si>
+  <si>
+    <t>Стояние на Угре</t>
+  </si>
+  <si>
+    <t>54°34′ с. ш. 36°03′ в. д.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A1%D1%82%D0%BE%D1%8F%D0%BD%D0%B8%D0%B5_%D0%BD%D0%B0_%D1%80%D0%B5%D0%BA%D0%B5_%D0%A3%D0%B3%D1%80%D0%B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Для тех, кто наблюдал со стороны за тем, как оба войска почти одновременно (в течение двух дней) повернули вспять, не доведя дело до решающей битвы, это событие казалось либо странным, мистическим, либо получало упрощённое объяснение: противники испугались друг друга, опасаясь принять сражение. На Руси же современники приписывали это чудесному заступничеству Богородицы, которая спасла Русскую землю от разорения. Видимо и поэтому реку Угру стали называть «поясом Богородицы». Великий князь Иван III со всем воинством вернулся в Москву, «и возрадовашася, и возвеселишася все людие радостию велиею зело». </t>
+  </si>
+  <si>
+    <t>Куровское, Калужская обл</t>
+  </si>
+  <si>
+    <t>Иван IV Грозный становится первым российским царем</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В 1547 году великий князь московский Иван IV Грозный венчался на царство и стал, таким образом, первым российским царём[50]. Новый титул позволял занять существенно иную позицию в дипломатических сношениях с Западной Европой. Великокняжеский титул переводился как «великий герцог», титул же «царь» в иерархии стоял наравне с титулом император[51]. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перемирие было заключено 18 февраля 1537 года в Москве. По его условиям Гомельская волость официально отходила Великому княжеству Литовскому, а крепости Себеж, Велиж и Заволочье, основанные русскими на завоёванной литовской территории, оставались в Русском государстве. 
+По мнению М. М. Крома, война 1534—1537 годов выявила растущую слабость военной организации Великого княжества Литовского и усиление его зависимости в оборонной сфере от помощи соседней Польши
+</t>
+  </si>
+  <si>
+    <t>Велиж</t>
+  </si>
+  <si>
+    <t>Русско-Литовская война</t>
+  </si>
+  <si>
+    <t>Казань</t>
+  </si>
+  <si>
+    <t>Астрахань</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> В походе участвовало 150-тысячное русское войско, вооружение включало 150 пушек. Казанский кремль был взят штурмом. Хан Едигер-Магмет был захвачен русскими воеводами[61]. Летописец зафиксировал: «На себя же государь не велел имати ни единыя медницы (то есть ни единого гроша), ни плену, токмо единого царя Едигер-Магмета и знамёна царские да пушки градские»[</t>
+  </si>
+  <si>
+    <t>Взятие Казани</t>
+  </si>
+  <si>
+    <t>Взятие Астрахани</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%98%D0%B2%D0%B0%D0%BD_%D0%93%D1%80%D0%BE%D0%B7%D0%BD%D1%8B%D0%B9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В результате этого похода Астраханское ханство было подчинено Русскому царству. 
+В 1556 году разрушена столица Золотой Орды Сарáй-Бату́. 
+После покорения Астрахани русское влияние стало простираться до Кавказа. В 1559 году князья Пятигорские и Черкасские просили Ивана IV прислать им отряд для защиты против набегов крымских татар и священников для поддержания веры; царь послал им двух воевод и священников, которые обновили павшие древние церкви, а в Кабарде проявили широкую миссионерскую деятельность, крестив многих в православие
+</t>
+  </si>
+  <si>
+    <t>Ливонская война</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9B%D0%B8%D0%B2%D0%BE%D0%BD%D1%81%D0%BA%D0%B0%D1%8F_%D0%B2%D0%BE%D0%B9%D0%BD%D0%B0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">К 1576 г Россия успешно захватила большие территории, - современные Латвию и Эстонию за исключением Риги и Ревеля, но сначала Польша, а затем Швеция (1579) выступили против России. 
+Ливонская конфедерация перестала существовать. Её территории перешли к Швеции, Дании и возникшему во время войны Польско-Литовскому государству — Речи Посполитой. 
+Русь была разорена, а северо-западные районы обезлюдели. Следует отметить и тот факт, что на ход войны и её итоги повлияли крымские набеги: из 25 лет войны в течение только на протяжении трёх лет не было значительных крымских набегов. 
+</t>
+  </si>
+  <si>
+    <t>Рига</t>
+  </si>
+  <si>
+    <t>Сожжение Москвы крымским ханом Давлет-Гиреем</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Итог похода: убиты десятки тысяч русских, более 150 тысяч уведены в рабство. После этого Девлет Герай отправил к царю Ивану Грозному посольство, требуя передачи ему Казани и Астрахани. Видя, что положение критическое, Иван Грозный предложил передать Девлету Гераю Астраханское ханство. Однако, хан отказался, считая, что теперь можно подчинить всё Русское государство. </t>
+  </si>
+  <si>
+    <t>1572 году, получив поддержку Османской империи, Девлет I Герай собрал для нового похода на русские земли 120-тысячную армию: 80 тысяч крымцев и ногайцев, 33 тысячи турок, 7 тысяч турецких янычар. В конце июля крымская орда подошла к Серпухову, разбила небольшие русские заставы и переправилась через реку Оку. По серпуховской дороге Девлет Герай двинулся к Москве. Русские воеводы, стоявшие с полками в Серпухове, Тарусе, Калуге, Кашире и Лопасне, выступили к Москве вслед за крымским войском, отрезая ему пути к отступлению. 30 июля — 2 августа 1572 года на реке Пахре, в 50 км от Москвы крымско-османская армия была уничтожена 25-тысячным русским войском под командованием князей Михаила Ивановича Воротынского и Дмитрия Ивановича Хворостинина в битве при Молодях. В боях крымцы и турки понесли огромные людские потери, был взят в плен знаменитый крымский военачальник Дивей-мурза, погиб ногайский мурза Теребердей. Среди погибших оказались сыновья хана, царевичи Шардан Герай и Хаспулад Герай</t>
+  </si>
+  <si>
+    <t>55°16′55″ с. ш. 37°31′44″ в. Д.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%94%D0%B5%D0%B2%D0%BB%D0%B5%D1%82_I_%D0%93%D0%B5%D1%80%D0%B0%D0%B9</t>
+  </si>
+  <si>
+    <t>Битва при Молодях</t>
+  </si>
+  <si>
+    <t>В 1589 году учреждён Московский патриархат, избран первый патриарх Иов</t>
+  </si>
+  <si>
+    <t>Учреждение Московского патриархата</t>
+  </si>
+  <si>
+    <t>Покорение Сибири Ермаком</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лишь весной 1582 года по рекам Жеравле, Баранче и Тагилу казаки выплыли в Туру. Они дважды разбили сибирских татар, на Туре и в устье Тавды. Кучум выслал против казаков Маметкула, с большим войском, но 1 августа и это войско было разбито Ермаком на берегу Тобола, при урочище Бабасаны. Наконец, на Иртыше, под Чувашевым, казаки нанесли окончательное поражение татарам в битве на Чувашевом мысу. Кучум оставил засеку, защищавшую главный город его ханства, Сибирь, и бежал на юг, в Ишимские степи. 
+26 октября (5 ноября) 1582 года Ермак вступил в покинутый татарами город Сибирь (Кашлык)[16]. Через четыре дня ханты с реки Демьянки, правого притока нижнего Иртыша, привезли в дар казакам пушнину и съестные припасы, главным образом рыбу. Ермак «лаской и приветом» встретил их и отпустил «с честью». 
+</t>
+  </si>
+  <si>
+    <t>Кашлык (Тобольск)</t>
+  </si>
+  <si>
+    <t>58°08′57″ с. ш. 68°31′10″ в. д.</t>
+  </si>
+  <si>
+    <t>30/06/1605</t>
+  </si>
+  <si>
+    <t>Вступление в Москву Лжедимитрия 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Царствование Лжедмитрия было ознаменовано ориентацией на Польшу и некоторыми попытками реформ. Не всё московское боярство признало Лжедмитрия законным правителем. Почти сразу по прибытии его в Москву князь Василий Шуйский через посредников начал распространять слухи о самозванстве. Воевода Пётр Басманов раскрыл заговор, и 23 июня (3 июля) 1605 года Шуйского схватили и осудили на смерть, помиловав лишь непосредственно у плахи. 
+На свою сторону Шуйский привлёк князей В. В. Голицына и И. С. Куракина. Заручившись поддержкой стоявшего под Москвой новгородско-псковского отряда, который готовился к походу на Крым, Шуйский организовал переворот. 
+В ночь с 16 на 17 (27) мая 1606 года боярская оппозиция, воспользовавшись озлоблением москвичей против явившихся в Москву на свадьбу Лжедмитрия польских авантюристов, подняла восстание, в ходе которого самозванец был жестоко убит[8]. Приход к власти представителя суздальской ветви Рюриковичей боярина Василия Шуйского не принёс успокоения
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A1%D0%BC%D1%83%D1%82%D0%BD%D0%BE%D0%B5_%D0%B2%D1%80%D0%B5%D0%BC%D1%8F</t>
+  </si>
+  <si>
+    <t>1/11/1612</t>
+  </si>
+  <si>
+    <t>Освобождение Москвы ополчением Минина и Пожарского</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В Кремле укрылись и изменники-бояре со своими семьями. Среди них находился в Кремле и ещё мало кому известный в то время племянник члена Семибоярщины и сын тушинского патриарха Михаил Романов со своею матерью Марфой Ивановной. Зная, что осаждённые поляки терпят страшный голод, Пожарский в конце сентября 1612 года направил им письмо, в котором предлагал польскому гарнизону сдаться. «Ваши головы и жизнь будут сохранены вам, — писал он, — я возьму это на свою душу и упрошу согласия на это всех ратных людей». На это последовал высокомерный отказ. 
+22 октября (1 ноября) 1612 года Китай-город был взят приступом русскими войсками
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%92%D1%82%D0%BE%D1%80%D0%BE%D0%B5_%D0%BD%D0%B0%D1%80%D0%BE%D0%B4%D0%BD%D0%BE%D0%B5_%D0%BE%D0%BF%D0%BE%D0%BB%D1%87%D0%B5%D0%BD%D0%B8%D0%B5</t>
+  </si>
+  <si>
+    <t>Для борьбы с последствиями Смуты был созван Земский собор 1613 года, на котором на царство был призван Михаил Романов — первый из династии Романовых, который через свою родственницу Анастасию Романову (первую жену Ивана Грозного) являлся ближайшим родственником угасшей династии Рюриковичей. Также он был «выгодным царём» для бояр, поскольку юноша, изначально не желавший нести бремя власти, мог легко стать игрушкой в руках бояр, которые в итоге фактически и правили</t>
+  </si>
+  <si>
+    <t>Избрание Михаила Романова на царство</t>
+  </si>
+  <si>
+    <t>Переяславль</t>
+  </si>
+  <si>
+    <t>10/01/1654</t>
+  </si>
+  <si>
+    <t>Переяславская Рада</t>
+  </si>
+  <si>
+    <t xml:space="preserve">согласно данным русского посольства, присягу дали 127 328 казаков, мещан и вольных войсковых селян (женщины и холопы к присяге не приводились). 
+Отказались присягать из православных лишь сторонники бывшего наказного гетмана Барабаша, назначенного польским правительством, утопленного реестровыми казаками вместе с другими шляхетскими начальниками, сторонниками панской власти, в битве под Жёлтыми Водами[9], у которого Хмельницкому удалось ранее хитростью выманить королевскую грамоту, которую тот использовал как прикрытие для сбора войск
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9F%D0%B5%D1%80%D0%B5%D1%8F%D1%81%D0%BB%D0%B0%D0%B2%D1%81%D0%BA%D0%B0%D1%8F_%D1%80%D0%B0%D0%B4%D0%B0</t>
+  </si>
+  <si>
+    <t>Реформа Патриарха Тихона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В ходе реформы богослужебная традиция была изменена в следующих пунктах: 
+1.Широкомасштабная «книжная справа», выразившаяся в редактировании текстов Священного Писания и богослужебных книг, которая привела к изменениям в славянских переводов некоторых текстов, в частности Символа веры: изъят союз «а» в словах о вере в Сына Божия «рождена, а не сотворена», о Царствии Божием стали говорить в будущем («не будет конца»), а не в настоящем времени («несть конца»), из 8-го члена, говорящего о вере в «Духа Святаго», исключено слово «Истиннаго». Было внесено множество других незначительных изменений, например, в имя «Ісус» (под титлом «Ic») была добавлена ещё одна буква и оно стало писаться «Іисус» (под титлом «Іис»).
+2.Замена двуперстного крестного знамения трёхперстным и отмена «метаний», или малых земных поклонов — в 1653 году Никон разослал по всем церквям московским «память», в которой говорилось: «не подобает в церкви метания творити на колену, но в пояс бы вам творити поклоны; ещё и тремя персты бы есте крестились».
+3.Крестные ходы Никон распорядился проводить в обратном направлении (против солнца, а не посолонь).
+4.Возглас «аллилуйя» во время богослужения стали произносить не дважды (сугубая аллилуйя), а трижды (трегубая).
+5.Изменено число просфор на проскомидии и начертание печати на просфорах.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D0%B0%D1%81%D0%BA%D0%BE%D0%BB_%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%BE%D0%B9_%D1%86%D0%B5%D1%80%D0%BA%D0%B2%D0%B8</t>
+  </si>
+  <si>
+    <t>Восстание Степана Разина</t>
+  </si>
+  <si>
+    <t>Царицын</t>
+  </si>
+  <si>
+    <t>Крестья́нская война́ 1667—1671, — война в России между войсками крестьян и казаков под предводи́тельством Степана Разина и царскими войсками. Окончилась поражением восставших.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%92%D0%BE%D1%81%D1%81%D1%82%D0%B0%D0%BD%D0%B8%D0%B5_%D0%A0%D0%B0%D0%B7%D0%B8%D0%BD%D0%B0</t>
+  </si>
+  <si>
+    <t>Не́рчинский договор — мирный договор между Русским царством и Империей Цин, впервые определивший отношения и границу между двумя государствами. Заключён 27 августа (6 сентября) 1689 года у Нерчинска.</t>
+  </si>
+  <si>
+    <t>Нерчин</t>
+  </si>
+  <si>
+    <t>Первый Русско-Китайский мирный договор</t>
+  </si>
+  <si>
+    <t>27/08/1689</t>
+  </si>
+  <si>
+    <t>Белгород</t>
+  </si>
+  <si>
+    <t>Русско-турецкая война</t>
+  </si>
+  <si>
+    <t xml:space="preserve">война Русского царства с Османской империей и вассальным ему Крымским ханством во время царствования Алексея Михайловича и Фёдора Алексеевича. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%A0%D1%83%D1%81%D1%81%D0%BA%D0%BE-%D1%82%D1%83%D1%80%D0%B5%D1%86%D0%BA%D0%B0%D1%8F_%D0%B2%D0%BE%D0%B9%D0%BD%D0%B0_(1672%E2%80%941681)</t>
+  </si>
+  <si>
+    <t>В 1689 году царевна Софья была свергнута Петром I и заключена в монастырь. Пётр стал единоличным правителем (с учётом недееспособности его брата соправителя Ивана V, умершего в 1696 году).</t>
+  </si>
+  <si>
+    <t>Начало царствования Петра I</t>
+  </si>
+  <si>
+    <t>Азов</t>
+  </si>
+  <si>
+    <t>Захват крепости Азов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В мае 1696 года 40-тысячная русская армия под командованием генералиссимуса Шеина вновь осадила Азов, только на этот раз русская флотилия блокировала крепость с моря. Пётр I принимал участие в осаде в звании капитана на галере. Не дожидаясь штурма, 19 (29) июля 1696 года крепость сдалась. Так был открыт первый выход России в южные моря. 
+Результатом Азовских походов стал захват крепости Азов, начало строительства порта Таганрог, возможность нападения на полуостров Крым с моря, что значительно обезопасило южные границы России
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/%D0%9F%D1%91%D1%82%D1%80_I</t>
   </si>
 </sst>
 </file>
@@ -1780,12 +2140,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1801,7 +2167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1819,6 +2185,9 @@
       <alignment vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2126,13 +2495,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J95"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B120" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A96" sqref="A96"/>
+      <selection pane="bottomRight" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -4498,6 +4867,562 @@
       </c>
       <c r="J95" s="3" t="s">
         <v>488</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="139.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B96" s="3">
+        <v>862</v>
+      </c>
+      <c r="D96" s="5"/>
+      <c r="E96" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="I96" s="3">
+        <v>1</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="279" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B97" s="3">
+        <v>911</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="I97" s="3">
+        <v>1</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="B98" s="3">
+        <v>988</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="232.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="B99" s="3">
+        <v>1016</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="232.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="B100" s="7">
+        <v>1237</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1240</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="B101" s="3">
+        <v>1240</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="139.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1362</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="279" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B103" s="3">
+        <v>1380</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="93" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B104" s="3">
+        <v>1471</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="G104" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="186" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="B105" s="7">
+        <v>1480</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="H105" s="3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1534</v>
+      </c>
+      <c r="C106" s="3">
+        <v>1537</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="G106" s="4"/>
+    </row>
+    <row r="107" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B107" s="3">
+        <v>1547</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="B108" s="3">
+        <v>1552</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="209.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="B109" s="3">
+        <v>1554</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="255.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="B110" s="3">
+        <v>1558</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1583</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="116.25" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B111" s="3">
+        <v>1571</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="325.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B112" s="3">
+        <v>1572</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="279" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="B113" s="3">
+        <v>1583</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="3" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B114" s="3">
+        <v>1589</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="F114" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="395.25" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B115" s="3">
+        <v>1605</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="F115" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="255.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B116" s="3">
+        <v>1612</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="162.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B117" s="3">
+        <v>1613</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="232.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="B118" s="3">
+        <v>1654</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B119" s="3">
+        <v>1654</v>
+      </c>
+      <c r="C119" s="3">
+        <v>1665</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B120" s="3">
+        <v>1670</v>
+      </c>
+      <c r="C120" s="3">
+        <v>1671</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1689</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="B122" s="3">
+        <v>1682</v>
+      </c>
+      <c r="C122" s="3">
+        <v>1681</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="69.75" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="B123" s="3">
+        <v>1689</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="232.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="B124" s="3">
+        <v>1696</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -4592,9 +5517,33 @@
     <hyperlink ref="G93" r:id="rId83"/>
     <hyperlink ref="G94" r:id="rId84"/>
     <hyperlink ref="G95" r:id="rId85"/>
+    <hyperlink ref="G97" r:id="rId86"/>
+    <hyperlink ref="G96" r:id="rId87"/>
+    <hyperlink ref="G98" r:id="rId88"/>
+    <hyperlink ref="G99" r:id="rId89"/>
+    <hyperlink ref="G100" r:id="rId90"/>
+    <hyperlink ref="G101" r:id="rId91"/>
+    <hyperlink ref="G102" r:id="rId92"/>
+    <hyperlink ref="G103" r:id="rId93"/>
+    <hyperlink ref="G104" r:id="rId94"/>
+    <hyperlink ref="G105" r:id="rId95"/>
+    <hyperlink ref="G107" r:id="rId96"/>
+    <hyperlink ref="G110" r:id="rId97"/>
+    <hyperlink ref="G112" r:id="rId98"/>
+    <hyperlink ref="G114" r:id="rId99"/>
+    <hyperlink ref="G115" r:id="rId100"/>
+    <hyperlink ref="G116" r:id="rId101"/>
+    <hyperlink ref="G117" r:id="rId102"/>
+    <hyperlink ref="G118" r:id="rId103"/>
+    <hyperlink ref="G119" r:id="rId104"/>
+    <hyperlink ref="G120" r:id="rId105"/>
+    <hyperlink ref="G121" r:id="rId106"/>
+    <hyperlink ref="G122" r:id="rId107"/>
+    <hyperlink ref="G123" r:id="rId108"/>
+    <hyperlink ref="G124" r:id="rId109"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId86"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId110"/>
 </worksheet>
 </file>
 

</xml_diff>